<commit_message>
tamaño botones de tareas arreglado
</commit_message>
<xml_diff>
--- a/Excel_tareas.xlsx
+++ b/Excel_tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacoc\Akali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4146E5BB-B304-459B-8850-C0A439952879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0299DA6-6EF3-4ACA-B4F8-CF67B402DE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" xr2:uid="{58A3BA58-A805-4B3F-98FC-E9854B22FB4B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="129">
   <si>
     <t>Nº 1 Autenticación y perfil de hábitos</t>
   </si>
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD407E0E-BF19-42C9-9C99-4C8BD6E0A35A}">
   <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2403,7 +2403,9 @@
       <c r="B72" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="2"/>
+      <c r="C72" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="D72" s="2">
         <v>0.5</v>
       </c>
@@ -2427,12 +2429,14 @@
       <c r="B73" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="2"/>
+      <c r="C73" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="D73" s="2">
         <v>1</v>
       </c>
       <c r="E73" s="33">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F73" s="44" t="s">
         <v>38</v>
@@ -2464,19 +2468,21 @@
       </c>
       <c r="I74" s="25"/>
     </row>
-    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C75" s="2"/>
+      <c r="C75" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="33">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F75" s="44" t="s">
         <v>38</v>
@@ -3426,7 +3432,7 @@
       </c>
       <c r="D2" s="33">
         <f>SUMIFS(TAREAS!$E$2:$E$338,TAREAS!$B$2:$B$338,"*"&amp;$A2&amp;"*",TAREAS!$F$2:$F$338,D$1) + SUMIFS('TAREAS EXTRA'!$E$4:$E$336,'TAREAS EXTRA'!$B$4:$B$336,"*"&amp;$A2&amp;"*",'TAREAS EXTRA'!$F$4:$F$336,D$1)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="33">
         <f>SUMIFS(TAREAS!$E$2:$E$338,TAREAS!$B$2:$B$338,"*"&amp;$A2&amp;"*",TAREAS!$F$2:$F$338,E$1) + SUMIFS('TAREAS EXTRA'!$E$4:$E$336,'TAREAS EXTRA'!$B$4:$B$336,"*"&amp;$A2&amp;"*",'TAREAS EXTRA'!$F$4:$F$336,E$1)</f>
@@ -3478,7 +3484,7 @@
       </c>
       <c r="Q2" s="83">
         <f>SUM(B2:P2)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -3840,7 +3846,7 @@
       </c>
       <c r="D8" s="83">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" s="83">
         <f t="shared" si="1"/>
@@ -3892,7 +3898,7 @@
       </c>
       <c r="Q8" s="83">
         <f>SUM(Q2:Q7)</f>
-        <v>82.75</v>
+        <v>84.75</v>
       </c>
     </row>
   </sheetData>
@@ -3902,23 +3908,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ac76a8e4-229b-45b3-bca1-87e9f4b60bc4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A2890032ECC8D42A9B47FCAB7A6AE5B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4bc73805db26cd76b1f507433ce02467">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac76a8e4-229b-45b3-bca1-87e9f4b60bc4" xmlns:ns4="445ad1ed-65e8-4ac6-89a2-5a80de8ff027" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85b08b0a29ea0cd8c42482704c8b3285" ns3:_="" ns4:_="">
     <xsd:import namespace="ac76a8e4-229b-45b3-bca1-87e9f4b60bc4"/>
@@ -4139,25 +4128,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787386DB-8B0E-416C-B49A-CF788B487C65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ac76a8e4-229b-45b3-bca1-87e9f4b60bc4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89206744-1C12-4D7A-BD24-E06D4EEE600C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ac76a8e4-229b-45b3-bca1-87e9f4b60bc4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B78835B5-62B6-4031-B516-2848BCFD4AA5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4174,4 +4162,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89206744-1C12-4D7A-BD24-E06D4EEE600C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ac76a8e4-229b-45b3-bca1-87e9f4b60bc4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787386DB-8B0E-416C-B49A-CF788B487C65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>